<commit_message>
- rowformat -> cellformat - colonne ETAT non barré - A valider sans URGENT ou RAPPEL
</commit_message>
<xml_diff>
--- a/inst/template/BEUBOIS_CR.xlsx
+++ b/inst/template/BEUBOIS_CR.xlsx
@@ -2159,8 +2159,8 @@
   </sheetPr>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Gros commit: - ajout perpare_cr et compile_cr - fichier excel pour photos - retaillage seulement photos incluses avec messages - read.r export.r -> xl.r - cr_config.r -> config.r - cr_reunion.rnw -> chantier_cr.rnw - renommages variables, eg: num_reu -> num
</commit_message>
<xml_diff>
--- a/inst/template/BEUBOIS_CR.xlsx
+++ b/inst/template/BEUBOIS_CR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="182" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="329" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LEGENDE" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,6 @@
     <sheet name="CEJOUR" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="PLANS" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="PLANSNOTE" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="PHOTOS" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">TACHES!$A$1:$G$251</definedName>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="651">
   <si>
     <t>CLE</t>
   </si>
@@ -1993,60 +1992,6 @@
   </si>
   <si>
     <t>Pour déposer des fichiers aller dans le dossier « 0\_Dépôts » et remplir le formulaire. Un mail notifiant le dépôt d'un élément doit nous être transmis.</t>
-  </si>
-  <si>
-    <t>FICHIER</t>
-  </si>
-  <si>
-    <t>COMMENTAIRE</t>
-  </si>
-  <si>
-    <t>P1010815.JPG</t>
-  </si>
-  <si>
-    <t>Enduit de l'imposte des fenêtres centrale de La Source par Grnunenwald</t>
-  </si>
-  <si>
-    <t>P1010816.JPG</t>
-  </si>
-  <si>
-    <t>Pose de l'ascenseur de la Source en cours par Schindler</t>
-  </si>
-  <si>
-    <t>P1010820.JPG</t>
-  </si>
-  <si>
-    <t>Reprise en sous œuvre de l'Epilobe par bari</t>
-  </si>
-  <si>
-    <t>P1010821.JPG</t>
-  </si>
-  <si>
-    <t>Préparation du coffrage de dalle de l'Epilobe par Bari</t>
-  </si>
-  <si>
-    <t>P1010822.JPG</t>
-  </si>
-  <si>
-    <t>Décoffrage dalle par Bari Epilobe</t>
-  </si>
-  <si>
-    <t>P1010823.JPG</t>
-  </si>
-  <si>
-    <t>Tranchée de raccordement Epilobe par Bari</t>
-  </si>
-  <si>
-    <t>P1010824.JPG</t>
-  </si>
-  <si>
-    <t>Menuiseries intérieures dans La Source par Chiodetti</t>
-  </si>
-  <si>
-    <t>P1010826.JPG</t>
-  </si>
-  <si>
-    <t>Mise en place des structures de faux plafond démontable dans La Source par Bari</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2104,7 @@
   </sheetPr>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -10224,7 +10169,7 @@
   </sheetPr>
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -10277,104 +10222,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9028340080972"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.5748987854251"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>651</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>653</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>655</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>657</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>659</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>661</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>663</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>665</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>667</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>668</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
DATE -> REUNION DATEREALISATIOn -> REALISATION
</commit_message>
<xml_diff>
--- a/inst/template/BEUBOIS_CR.xlsx
+++ b/inst/template/BEUBOIS_CR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="329" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="165" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LEGENDE" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="652">
   <si>
     <t>CLE</t>
   </si>
@@ -932,928 +932,931 @@
     <t>03 DETAILS</t>
   </si>
   <si>
+    <t>REUNION</t>
+  </si>
+  <si>
+    <t>ECHEANCE</t>
+  </si>
+  <si>
+    <t>REALISATION</t>
+  </si>
+  <si>
+    <t>PRIORITE</t>
+  </si>
+  <si>
+    <t>ETAT</t>
+  </si>
+  <si>
+    <t>SECTION</t>
+  </si>
+  <si>
+    <t>ACTEUR</t>
+  </si>
+  <si>
+    <t>TACHE</t>
+  </si>
+  <si>
+    <t>URGENT</t>
+  </si>
+  <si>
+    <t>epb</t>
+  </si>
+  <si>
+    <t>alf</t>
+  </si>
+  <si>
+    <t>Teinte menuiserie à proposer - gris ardoise / gris anthracite. Proposer une tôlerie assortie à l'architecte</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>Débuter votre intervention par la pose des menuiseries du 1er niveau façade Nord pour permettre une sécurisation de l'accès</t>
+  </si>
+  <si>
+    <t>Dernier délais pour pose des tablettes + menuiseries sud car le lot ITE ainsi que le second \oe uvre du RDC sont bloqués depuis trop longtemps</t>
+  </si>
+  <si>
+    <t>barigo</t>
+  </si>
+  <si>
+    <t>Poursuivre les travaux de terrassement dans la chaufferie + mise en place des réseaux enterrés (compris fourreaux réseau de chaleur en 250 + regard réseau de chaleur + réaliser réseau évacuation dans l'extension des sanitaires.</t>
+  </si>
+  <si>
+    <t>Réaliser le GO de la chaufferie e le GO de  l'extension des sanitaires</t>
+  </si>
+  <si>
+    <t>Etayer pilier Sud-Ouest en amont de la démolition du pignon</t>
+  </si>
+  <si>
+    <t>La réalisation du cuvelage (étanchéité) de la fosse d'ascenseur est à votre lot</t>
+  </si>
+  <si>
+    <t>Intervention de l'ascensoriste prévue à partir du 15 Juillet. Le cuvelage de la fosse doit impérativement être terminé à cette date pour permettre à ce dernier de travailler</t>
+  </si>
+  <si>
+    <t>La chape de La Source va être poncer le 09 Juillet. Débarasser le RDC pour permettre son intervention</t>
+  </si>
+  <si>
+    <t>tav</t>
+  </si>
+  <si>
+    <t>Prévoir intervention sur la maison du gardien pour découper la casquette existante.</t>
+  </si>
+  <si>
+    <t>orga</t>
+  </si>
+  <si>
+    <t>belc</t>
+  </si>
+  <si>
+    <t>Faire un récap sous forme de canevas des prestations prévues au titre des courants faibles sur le site</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>Suite à la réception du plan EXE R+2 Tavaillon, poursuivre vos études</t>
+  </si>
+  <si>
+    <t>Suite à la réception du plan EXE R+3 Tavaillon, poursuivre vos études</t>
+  </si>
+  <si>
+    <t>Il semblerait que les plans transmis à Bari pour la chaufferie ne contiennent pas les réservations transmises par le lot CVC. Mettre à jour.</t>
+  </si>
+  <si>
+    <t>beth</t>
+  </si>
+  <si>
+    <t>Suite à la réunion du technique du 18 Juin, diffuser le nouveau schéma hydraulique.</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>Travaux hors marché : surélever de 10cm la porte provisoire située à l'ouest du bâtiment au RDC bas, la porte qui barre l'accès aux étages</t>
+  </si>
+  <si>
+    <t>Pose des menuiseries intérieures</t>
+  </si>
+  <si>
+    <t>ecp</t>
+  </si>
+  <si>
+    <t>Démontage échaffaudage sur 7 travées à prévoir pour Mercredi 15/07.</t>
+  </si>
+  <si>
+    <t>el2</t>
+  </si>
+  <si>
+    <t>Déplacement des espaces d'attente sécurisés selon plans à paraître semaine prochaine. Prendre dispositions en conséquence.</t>
+  </si>
+  <si>
+    <t>moe</t>
+  </si>
+  <si>
+    <t>Transmettre côte pour baie perpendiculaire à l'escalier au R+1 les Sources</t>
+  </si>
+  <si>
+    <t>L'échaffaudage étant installé, prévoir la dépose du paratonerre.</t>
+  </si>
+  <si>
+    <t>La chape de La Source va être poncer le 09 Juillet. Débarasser le RDC bas pour permettre son intervention</t>
+  </si>
+  <si>
+    <t>Prévoir intervention sur la maison du gardien pour les modifications en façade (coffret force / lumière)</t>
+  </si>
+  <si>
+    <t>grw</t>
+  </si>
+  <si>
+    <t>L'isolation du RDC de l'Epilobe, depuis l'extérieur (dans les locaux condamnés) peut être prévue. Epaisseur à prévoir : 12 cm de polystyrène, isolation des murs et des plafonds</t>
+  </si>
+  <si>
+    <t>Intervenir pour mettre en place isolant entre menuiseries et avant toît au R+1 avant le démontage de l'échaffaudage jusqu'à la finition extérieure</t>
+  </si>
+  <si>
+    <t>Terminer enduit au dessus des menuiseries des travées centrales pour le Mercredi 15/07, date de démontage de l'échaffaudage</t>
+  </si>
+  <si>
+    <t>Donner emplacement bouche incendie à Parolini</t>
+  </si>
+  <si>
+    <t>gst</t>
+  </si>
+  <si>
+    <t>Intervention pour réalisation des plafonds démontables. Commencer par RDC Haut et R+1 salle situées au Sud - attendre intervention de l'électricien pour intervention dans les circulations Nord  des niveaux supérieurs et le RDC Bas</t>
+  </si>
+  <si>
+    <t>htz</t>
+  </si>
+  <si>
+    <t>La chape de La Source va être poncer le 09 Juillet. Débarasser le RDC bas pour permettre son intervention + programmer intervention à la suite</t>
+  </si>
+  <si>
+    <t>RAPPEL</t>
+  </si>
+  <si>
+    <t>Vous rapprocher de M Million pour organiser la livraison de la paille</t>
+  </si>
+  <si>
+    <t>laem</t>
+  </si>
+  <si>
+    <t>Intervention serrurerie pour pergolas</t>
+  </si>
+  <si>
+    <t>Programmer découpe partielle de l'escalier métallique existant sur la maison du gardien.</t>
+  </si>
+  <si>
+    <t>ldr</t>
+  </si>
+  <si>
+    <t>L'espace compris entre la volée ascendante de marche et la cloison construite dans l'escalier doit être colmatter par une "mini paillasse" en plâtre qui supportera du carelage</t>
+  </si>
+  <si>
+    <t>Travaux complémentaires plâtrerie, conformément aux crobarres transmis</t>
+  </si>
+  <si>
+    <t>Boucher les trous au plâtre pour permettre l'intervention de Gaistel</t>
+  </si>
+  <si>
+    <t>Mise en place doublage dans les cages d'escalier</t>
+  </si>
+  <si>
+    <t>Attention : vous êtes en retard sur les enduites de rebouchage de trous, le faux plafond démontable attend après vous</t>
+  </si>
+  <si>
+    <t>Vu sur site : encoffrer poutre métalique au RDC bas</t>
+  </si>
+  <si>
+    <t>mcb</t>
+  </si>
+  <si>
+    <t>Transmettre devis pour insufflation supplémentaire + frein-vapeur + contre-lattage sur 57 m$^2$ / épaisseur 13 cm dans l'Epilobe</t>
+  </si>
+  <si>
+    <t>Prévoir intervention pour soufflage ouate dans plancher bas R+2 à partir du 25 Mai - Reporté 08/06/2015</t>
+  </si>
+  <si>
+    <t>mil</t>
+  </si>
+  <si>
+    <t>Travaux sur MOB chaufferie à partir du 10 Aout 2015</t>
+  </si>
+  <si>
+    <t>Intervention sur la façade des sources pour mise en place bardage + casquettes brise soleil à partir du 22/07/2015</t>
+  </si>
+  <si>
+    <t>moa</t>
+  </si>
+  <si>
+    <t>Participer à la réunion du 27 Mars 14h00 pour finaliser l'appareillage électrique dans l'Epilobe</t>
+  </si>
+  <si>
+    <t>La réunion du 22 avec M Weulersse est déplacée à 15h</t>
+  </si>
+  <si>
+    <t>Fournir puissance électrique pour raccordement Auberge + Caprin</t>
+  </si>
+  <si>
+    <t>Terminer balance financière pour Parolini</t>
+  </si>
+  <si>
+    <t>Programmer test d'étanchéité à l'air + étanchéité à l'air des réseaux</t>
+  </si>
+  <si>
+    <t>Préciser architecture France Telecom + adduction d'eau bâtiment Epilobe.</t>
+  </si>
+  <si>
+    <t>Redessiner le réseau de chaleur</t>
+  </si>
+  <si>
+    <t>Une balance financière a été proposée par l'entreprise Million. Donner un avis et transmettre une proposition d'avenant à la Maîtrise d'Ouvrage</t>
+  </si>
+  <si>
+    <t>Reprendre le planning en intégrant les congés pour transmettre dates d'intervention à Million + transmettre planning OPC à la MOA</t>
+  </si>
+  <si>
+    <t>Mettre à jour plan réseau de chaleur</t>
+  </si>
+  <si>
+    <t>Transmettre plans à Chiodetti pour l'Epilobe (réservations)</t>
+  </si>
+  <si>
+    <t>Proposer un canevas pour fonctionnement Courants Faibles sur l'ensemble du site</t>
+  </si>
+  <si>
+    <t>Transmettre côtes de la limite préau sur la façade est pour que l'ITE puisse s'arrêter au bon endroit.</t>
+  </si>
+  <si>
+    <t>Réaliser un état des lieux général du chantier du point de vue financier intégrant toutes plus values / moins values connues à ce jour.</t>
+  </si>
+  <si>
+    <t>Préparer OS GO pour signature par le MOA</t>
+  </si>
+  <si>
+    <t>Contacter Eric Michel, chef des pompiers à Orbey, pour valider le principe de "réserve incendie"</t>
+  </si>
+  <si>
+    <t>La réunion du 22 avec M Barth et M Bourcard est déplacée à 15h</t>
+  </si>
+  <si>
+    <t>nic</t>
+  </si>
+  <si>
+    <t>Boucher les cheminées + mettre en place les fenêtre de toîts + déplacer la dalle de gouttière</t>
+  </si>
+  <si>
+    <t>Commander fenêtres de toît en triple vitrage</t>
+  </si>
+  <si>
+    <t>remplacement dalle de gouttière de la Source, façade Nord et Sud</t>
+  </si>
+  <si>
+    <t>Réaliser l'étanchéité des murs enterrés du RDC au Nord du Tavaillon</t>
+  </si>
+  <si>
+    <t>paro</t>
+  </si>
+  <si>
+    <t>Prévoir évacuations sous la boulangerie à partir du 18 Mai</t>
+  </si>
+  <si>
+    <t>Prévoir raccordement avaloir de la réserve situé au Nord niveau 0 de l'Epilobe vers le collecteur EU situé sous les WC.</t>
+  </si>
+  <si>
+    <t>Terrassement à prévoir sous la chaufferie à partir du 01 Juillet.</t>
+  </si>
+  <si>
+    <t>Devis à transmettre pour : travaux en supplément dans la chaufferie pour installation d'un regard + fourreaux pour raccordement du réseau de chaleur</t>
+  </si>
+  <si>
+    <t>Programmer de tirer une évacuation pour raccordement au réseau EU depuis sous-station SOURCE</t>
+  </si>
+  <si>
+    <t>Une canalisation d'eau a été endommagée, elle déverse sur l'échaffaudage ce qui ravine ses fondation. La manchonner en urgence pour que cessent les dégâts</t>
+  </si>
+  <si>
+    <t>Transmettre Bon de Livraisons pour justifier différence entre le calcul de l'architecte et vos mêtrés pour les travaux en plus value</t>
+  </si>
+  <si>
+    <t>phb</t>
+  </si>
+  <si>
+    <t>Transmettre les éléments de réservations manquant actuellement à ceux précédemment transmis : mur Est de la chaufferie contre bâtiment existant, VB, VH -  revoir emplacement cheminée.</t>
+  </si>
+  <si>
+    <t>Transmettre les réservations dans les parois de la chaufferie à Gettec, compris les réservations du mur Est de la chaufferie ainsi que la VB et la VH</t>
+  </si>
+  <si>
+    <t>Dès que la mise à jour des plans sera réalisée par l'architecte, prévoir de mettre en place les tubes d'alimentation chauffage pour les radiateurs R+2 de l'Epilobe</t>
+  </si>
+  <si>
+    <t>Prévoir commande CTA pour pose fin Mai</t>
+  </si>
+  <si>
+    <t>Programmer test étanchéité à l'air du réseau à la suite de votre intervention pour le 03 Juin</t>
+  </si>
+  <si>
+    <t>L'étanchéité à l'air des réseaux devra être renforcée : joint des gaines + mastic + ruban adhésif pour atteindre une classe d'étanchéité des réseaux correcte</t>
+  </si>
+  <si>
+    <t>Réaliser calfeutrement propre au plâtre pour réencoffrage des IPN.</t>
+  </si>
+  <si>
+    <t>Prévoir la mise en place de grilles prise d'air / rejet d'air sur le pignon Ouest du bâtiment + chiffrer la mise en place de grilles pour ventilation du comble perdus. Intervention urgente pour permettre au lot ITE de poursuivre.</t>
+  </si>
+  <si>
+    <t>Le plenum de la salle thérapie mesure 4 cm. Il est nécessaire de repasser les gaines dans la circulation.</t>
+  </si>
+  <si>
+    <t>Les registres d'équilibrage dans le réseau de La Source n'ont pas été mis en place. Prévoir leur mise en place.</t>
+  </si>
+  <si>
+    <t>Laquez les grilles extérieures en blanc selon RAL 9001</t>
+  </si>
+  <si>
+    <t>Transmettre réservations dans les Prémurs pour synthèse</t>
+  </si>
+  <si>
+    <t>Transmettre réservation dans R+2 suite à la diffusion des plans ARCHI EXE</t>
+  </si>
+  <si>
+    <t>Lors de votre intervention pour dépose et évacuation des chaudières de La Source et de L'Epilobe, vos équipes ont disqué des poteaux servant d'étendoir à linge hors de toute demande de la part de la maîtrise d'\oe uvre, à la suite de quoi des éléments métalliques émergents sont demeurés sur site, camouflés par la pelouse. Cette semaine, la société BARI a vu l'un de ses engins malheureusement creuver sur l'une de ces émergences. Constaté ce jour sur site 15/04/2015. Merci de vous rapprocher de la société BARI afin de trouver une solution à l'amiable à cet incident.</t>
+  </si>
+  <si>
+    <t>Transmettre réservation dans le R+3 suite à la diffusion des plans ARCHI EXE</t>
+  </si>
+  <si>
+    <t>URGENT : vous rapprocher de Bari pour intégrer ce qu'il faut dans les prémurs (alimentation radiateurs). Les prémurs sont en train d'être mis en place !</t>
+  </si>
+  <si>
+    <t>Dans la chaufferie, prévoir un raccordement dans un regard pour le réseau de chaleur</t>
+  </si>
+  <si>
+    <t>Programmer interventions pour réseau en dalle haute RDC pour le 13 Juillet 2015</t>
+  </si>
+  <si>
+    <t>sch</t>
+  </si>
+  <si>
+    <t>Les sujétions à votre installations concernant la tige fileté sur le mur Est de la cage d'ascenseur sont à votre charge. Si vous souhaitez sous-traite votre intervention à la société Bari, les contacter pour leur donner les instructions.</t>
+  </si>
+  <si>
+    <t>stm</t>
+  </si>
+  <si>
+    <t>tch</t>
+  </si>
+  <si>
+    <t>Ponçage de la chape programmé pour le 09/07/2015 - récupérer clé d'accès au chantier auprès de Nicolas Bourcard</t>
+  </si>
+  <si>
+    <t>ths</t>
+  </si>
+  <si>
+    <t>Mise en place réseaux + évacuations des logements R+2 Epilobe selon plans architectes transmis le 07/07/2015</t>
+  </si>
+  <si>
+    <t>vcz</t>
+  </si>
+  <si>
+    <t>Réaliser dossier administratif « demande de raccordement »</t>
+  </si>
+  <si>
+    <t>Finaliser la demande de raccordement ERDF</t>
+  </si>
+  <si>
+    <t>Le 23 Mars 2015, l'architecte va donner les instructions côtées au lot démolition sur site, notamment en relation avec le passage des réseaux. Transmettre éléments complémentaires au dossier Marché si  besoin</t>
+  </si>
+  <si>
+    <t>Diffusion plan de réservation Epilobe pour le 22/04/2015</t>
+  </si>
+  <si>
+    <t>Prévoir terrassement pour chaufferie à partir du 05/05/2015</t>
+  </si>
+  <si>
+    <t>Prévoir 1er intervention à partir du 18 Mai pour évacuation et alimentation des logements R+2 situés à l'intérieur du plancher en cours de construction</t>
+  </si>
+  <si>
+    <t>Intervention à prévoir à partir du 27 Mai - Reporté 03 Juin</t>
+  </si>
+  <si>
+    <t>Programmer interventions nécessaires en réseaux enterrés sous la chaufferie conjointement au travail du lot terrassement pour la semaine du 06 Juillet.</t>
+  </si>
+  <si>
+    <t>Prévoir jambe de force pour soutien des pannes</t>
+  </si>
+  <si>
+    <t>Prévoir de rehausser les pannes + faîtage</t>
+  </si>
+  <si>
+    <t>Programmer intervention pour réalisation de l'étanchéité contre les murs enterrés à partir du  13 Juillet 2015</t>
+  </si>
+  <si>
+    <t>et de l'Epilobe pour permettre à Bari de poursuivre son travail.</t>
+  </si>
+  <si>
+    <t>Tracer sur site les réservations dans l'Epilobe + La Source - RDV pris avec Bari</t>
+  </si>
+  <si>
+    <t>CHAUFFERIE : transmettre réservations à GETTEC</t>
+  </si>
+  <si>
+    <t>TS proposés pour Grunenwald : peinture sous face avant toît La Source- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Intervention à programmer pour réaliser les structure pare soleil de la façade pour mi-avril Début Mai.</t>
+  </si>
+  <si>
+    <t>Alimentation des radiateurs des circulations en apparents comme proposé validée</t>
+  </si>
+  <si>
+    <t>Sur 7 travées, l'échaffaudage devra être déplacé afin de se retrouver à 80 cm du mur. Aux abouts des travées restant "proche" de la façade, des équerres devront être fournies pour permettre au lot ITE de travailler (finitions sur casquettes bakélite). Votre intervention ne pourra se faire avant le 06 Juillet, car l'ITE doit, au préalable poser un isolant au dessus des menuiseries R+1 (sous l'avant toît qui deviendra inaccessible une fois les casquettes bakélites posées). Transmettre devis Travaux Supplémentaires.</t>
+  </si>
+  <si>
+    <t>Raccorder chauffe eau (celui en face à gauche dans la chaufferie) pour production ECS - attente eau</t>
+  </si>
+  <si>
+    <t>Vous coordoner avec Herrbach pour mettre en place le réseau de chaleur.</t>
+  </si>
+  <si>
+    <t>L'alimentation en eau de l'Epilobe se fera via la chaufferie et en tranchée commune avec le réseau de chaleur.</t>
+  </si>
+  <si>
+    <t>TS proposé à Herrbach : mise en place d'une liaison en réseau de chaleur entre l'auberge et Le Tavaillon- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Moins value proposée Parolini : suppression du réseau d'adduction spécifique incendie, vu avec le SDIS- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>transmission d'un devis par ECP pour lui permettre de démonter / remonter les 7 travées centrales d'échaffaudage au Sud, pour la mise en place des casquettes brise soleil.</t>
+  </si>
+  <si>
+    <t>transmission d'un devis par Nicolas R pour remplacement des dalles de gouttière du bâtiment la source</t>
+  </si>
+  <si>
+    <t>baridem</t>
+  </si>
+  <si>
+    <t>Ouverture tranchée pour évacuations RDC</t>
+  </si>
+  <si>
+    <t>Réalisation des travaux sur la boulangerie à partir 01 Juin 2015</t>
+  </si>
+  <si>
+    <t>Prévoir le renforcement de la fixation du portique métallique (actuellement fixé sur un lintaux qui va être détruit)</t>
+  </si>
+  <si>
+    <t>Finaliser votre intervention en liant la structure métallique à la façade. Le maçon attend après vous.</t>
+  </si>
+  <si>
+    <t>Fournir éléments complémentaires désenfumage</t>
+  </si>
+  <si>
+    <t>Donnez vos prescriptions pour améliorer l'étanchéité à l'air du système de désenfumage</t>
+  </si>
+  <si>
+    <t>Terminer balance financière pour Million</t>
+  </si>
+  <si>
+    <t>SOURCE : faire le point sur les poignées de portes intérieures / serrures moletées</t>
+  </si>
+  <si>
+    <t>Aboutir à une solution accepté par FIBE et le BCT pour les clapets d'étanchéité à l'air dans les gaines de désenfumage du Tavaillon</t>
+  </si>
+  <si>
+    <t>Validation du raccordement en 160 sur la conduite existante de diamètre 90 intérieur</t>
+  </si>
+  <si>
+    <t>Choisir teinte enduit de finition La Source - Urgent pour permettre au lot ITE de travailler.</t>
+  </si>
+  <si>
+    <t>Transmettre à Parolini : plans réseaux sous chaufferie, drains, plan chaufferie, plan GO</t>
+  </si>
+  <si>
+    <t>Vous rapprocher de Thomas Weulersse pour étudier une alternative en Zinc sur la maison du Gardien.</t>
+  </si>
+  <si>
+    <t>Le vide sanitaire de la maison du gardien est isolé par 3 cm de polystyrène. Vérifier que cela permette d'atteindre les exigences de la labellisation (en conservant également la toiture existante).</t>
+  </si>
+  <si>
+    <t>EPILOBE : Transmettre plans EXE à Theisen</t>
+  </si>
+  <si>
+    <t>Evacuer radiateurs vers ferrailleur comme vu sur site</t>
+  </si>
+  <si>
+    <t>Contacter France Telecom pour qu'ils nous communiquent leurs arrivées sur le site</t>
+  </si>
+  <si>
+    <t>Transmettre diamètres raccordement AEP à Parolini</t>
+  </si>
+  <si>
+    <t>Mettre à jour le plan des réseaux pour l'ensemble du site et le transmettre à Parolini et Muré</t>
+  </si>
+  <si>
+    <t>Déterminer avec Thomas le principe d'évacuation des EP du bâtiment - notamment, vérifier que le tube Coupé à l'Est du bâtiment n'est pas relié à la descente à l'angle Nord Est</t>
+  </si>
+  <si>
+    <t>Programmer l'intervention sur le bâtiment La Source pour le mois de Mai</t>
+  </si>
+  <si>
+    <t>Reprendre feuillures portes d'entrée du RDC haut</t>
+  </si>
+  <si>
+    <t>Travaux hors marché : fourniture et pose de 3 cylindres pour les portes provisoires</t>
+  </si>
+  <si>
+    <t>Lors de votre intervention, stocker proprement les garde-corps intérieurs de l'échaffaudage</t>
+  </si>
+  <si>
+    <t>Les tubes associés aux emplacements de radiateurs initiaux doivent être supprimer et bouchonnés.</t>
+  </si>
+  <si>
+    <t>Poursuivre votre intervention dans le bâtiment</t>
+  </si>
+  <si>
+    <t>Réaliser en priorité les travaux dans le WC du RDC bas pour permettre au carreleur de travailler</t>
+  </si>
+  <si>
+    <t>Réaliser une cloison provisoire au RDC bas, à droite de l'ascenseur pour sécuriser l'accès aux étages vis-à-vis du vol</t>
+  </si>
+  <si>
+    <t>Prioriser votre intervention sur les WC de l'ensemble des niveaux pour permettre au carreleur de travailler</t>
+  </si>
+  <si>
+    <t>1.5 cm à rattraper entre les menuiseries à l'est et celle au sud en mordant sur le chassis fixe situé à l'Est</t>
+  </si>
+  <si>
+    <t>L'échaffaudage va être démonter sur les 7 travées centrales, coordonner votre intervention pour mise en place de la pergola.</t>
+  </si>
+  <si>
+    <t>Programmer intervention pour ponçage de la chape</t>
+  </si>
+  <si>
+    <t>Réalisation cloisons provisoires au RDC bas et au RDC haut pour permettre la sécurisation du site - nota au RDC Bas, la cloison doit laisser un espace de 15 cm sous le plâtre pour permettre au carreleur de travailler</t>
+  </si>
+  <si>
+    <t>Remplacer chassis désenfumage R+1 par chassis fixe</t>
+  </si>
+  <si>
+    <t>Pour les menuiseries non posées (portes d'entrées Source) , poser l'isolant jusqu'à une distance de 50 cm de la menuiserie</t>
+  </si>
+  <si>
+    <t>Le rejet d'air a finalement été déplacé au RDC bas centré sur la fenêtre pour respecter une distance optimisée entre prise et rejet.</t>
+  </si>
+  <si>
+    <t>Confirmation : les réservations dans les cloisonnements intérieurs sont à votre charge.</t>
+  </si>
+  <si>
+    <t>Commander l'ascenseur pour pose à partir du 25/05/2015</t>
+  </si>
+  <si>
+    <t>Commander ascenceur pour pose à la mi Juin</t>
+  </si>
+  <si>
+    <t>Votre intervention peut débuter dans les étages.</t>
+  </si>
+  <si>
+    <t>L'eau chaude alimentant le lavoir devra être isolée.</t>
+  </si>
+  <si>
+    <t>Mettre en place les clôtures de chantier selon le PGC.</t>
+  </si>
+  <si>
+    <t>Transmettre réservation dans R+2</t>
+  </si>
+  <si>
+    <t>Réalisation des fondations</t>
+  </si>
+  <si>
+    <t>URGENT : vous rapprocher de Bari pour intégrer ce qu'il faut dans les prémurs (évacuations et éventuellement alimentation). Les prémurs sont en train d'être mis en place !</t>
+  </si>
+  <si>
+    <t>Le réseau de chaleur n'empruntant pas le même cheminement, réaliser le fanchissement du parking pour l'alimentation EF uniquement.</t>
+  </si>
+  <si>
+    <t>Poursuivre les travaux selon planning. Transmettre votre période de congé.</t>
+  </si>
+  <si>
+    <t>Transmettre dès réceptions des plans des prémurs vos incorporations</t>
+  </si>
+  <si>
+    <t>Prévoir intervention si vous avez des incorporations dans la dalle basse RDC dès la semaine prochaine</t>
+  </si>
+  <si>
+    <t>Les seuils des portes en granit doivent faire une hauteur de 7 cm.</t>
+  </si>
+  <si>
+    <t>5 menuiseries R+2 sur pignons Est et Ouest seront posées en applique intérieure</t>
+  </si>
+  <si>
+    <t>La double porte et la simple porte sur la façade sud sont inversées</t>
+  </si>
+  <si>
+    <t>Les fenêtres fixes sur les plans (R+1 Sud) sont effectivement fixes</t>
+  </si>
+  <si>
+    <t>Les fenêtres qui ne sont pas à votre marché (R+2) ne seront pas réalisées</t>
+  </si>
+  <si>
+    <t>La nouvelle fenêtre à l'Est RDC sera de type 2 OB - 1er ouvrant à gauche vu de  l'intérieur</t>
+  </si>
+  <si>
+    <t>La fenêtre situé au RDC à l'est sur le mur restant à construire sera de type pose en applique</t>
+  </si>
+  <si>
+    <t>Le bardage choisie est de type rainuré languette, largeur des lames : 18 cm (cf. photo en fin de compte-rendu)</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Interdiction d'accéder aux armoires électriques situées dans La Source : elles sont sous tension.</t>
+  </si>
+  <si>
+    <t>Seules les entreprises habilitées peuvent intervenir sur l'amiante, Interdiction notamment à toute entreprise non habilitée d'intervenir sur la couverture du bâtiment Epilobe</t>
+  </si>
+  <si>
+    <t>Des clés de la base-vie sont disponible auprès de M Dulau - se manifester</t>
+  </si>
+  <si>
+    <t>1 seule situation mensuelle est accepté, elle doit être transmise dernière semaine du mois pour validation lors de la première semaine du mois suivant</t>
+  </si>
+  <si>
+    <t>Le port du casque est obligatoire sur l'ensemble du chantier</t>
+  </si>
+  <si>
+    <t>Désormais, les factures transmises après la dernière semaine du mois ne seront traitées qu'à la fin du mois suivant par la maîtrise d'\oe uvre</t>
+  </si>
+  <si>
+    <t>Le RDC haut et le R+1 de La Source sont désormais condamnés. Des clés sont disponibles auprès de M Bourcard. Il est impératif de refermer le chantier chaque soir.</t>
+  </si>
+  <si>
+    <t>Le chemin sera coupé pendant 3 semaine au niveau des travaux de terrassement en chaufferie à partir du 15 Juillet</t>
+  </si>
+  <si>
+    <t>Plan EXE La Source : l'arrivée d'eau du bâtiment Source se fera dans le local sous station sous l'escalier</t>
+  </si>
+  <si>
+    <t>Etudier le détail d'alimentation des BSO au travers de la paille (sécurité ?) - le câble passe derrière le parement intérieur puis traverse la façade au niveau du lintau bois (à percer) au dessus de la fenêtre</t>
+  </si>
+  <si>
+    <t>Etudier le détail de l'alimentation des détecteurs de fumée situés en applique sous les faux plafonds coupe feu -  a priori  système de double plafond au R+3 et dalle brute dans les chambres donc pas de problème</t>
+  </si>
+  <si>
+    <t>Nota : leader platrerie sera en congé à partir du 24 Juillet</t>
+  </si>
+  <si>
+    <t>sps</t>
+  </si>
+  <si>
+    <t>Le poteau situé à proximité du bâtiment Les Caprins sera rapidement hors service et ce pour la durée du chantier</t>
+  </si>
+  <si>
+    <t>Le 04 Avril 2015, M Weulersse vous a notifié par mail le choix du modèle et de la teinte pour la protection solaire : Fundermax 3003 NT Rubinus Red - il est urgent de le mettre en commande - Rappel : l'échaffaudage sera installé durant 2 mois seulement</t>
+  </si>
+  <si>
+    <t>Le bardage doit être également commandé rapidement : bardage en mélèze sans teinte avec fibre verticale - Rappel : l'échaffaudage sera installé durant 2 mois seulement</t>
+  </si>
+  <si>
+    <t>Vous avez proposé une alternative à la solution proposé par Terranergie. Ceux-ci la refuse. Merci de mettre vos plans et vos commandes en cohérence avec les remarques du BET</t>
+  </si>
+  <si>
+    <t>Ventiler également les locaux bureau (soufflage 60 m3/h) + maintenance rangement/ RDC et reprise (60 m3/h)</t>
+  </si>
+  <si>
+    <t>Des plafonds type aléatoires '5/15/20' doivent être posés dans le hall d'entrée et dans la pièce thérapie au R+1</t>
+  </si>
+  <si>
+    <t>Poursuivre votre intervention - les menuiseries intérieures peuvent être posées dans les étages</t>
+  </si>
+  <si>
+    <t>Repose des radiateurs non habillés validé</t>
+  </si>
+  <si>
+    <t>Choix des teintes : peinture sous face avant toît RAL 3009 , crépis RAL 9001</t>
+  </si>
+  <si>
+    <t>Les portes au Nord seront à passage PMR ; le grand ouvrant sera aligner avec le couloir faisant face ; pas de traverse horizontale.</t>
+  </si>
+  <si>
+    <t>Confirmation : Sol fini = sol brut + 0.17m</t>
+  </si>
+  <si>
+    <t>La teinte choisi par la MOE et le MOA pour les menuiseries de la Source est KASTANIE selon nuancier proposé</t>
+  </si>
+  <si>
+    <t>Remettre en place les garde-corps intérieurs de l'échaffaudage à la suite de votre intervention</t>
+  </si>
+  <si>
+    <t>Soigner la mise en \oe uvre des vitrages, au silicone, sur les chassis fixes faite sur chantier. L'expérience montre que cela peut être des faiblesses en terme d'étanchéité à l'air</t>
+  </si>
+  <si>
+    <t>En raison du retard sur votre intervention dans le bâtiment des dispositions ont été prises pour fermer l'accès aux étages du bâtiment La Source.</t>
+  </si>
+  <si>
+    <t>ATTENTION : les revêtements des escaliers seront conservés, les protéger afin qu'ils ne soient pas abîmer par la démolition</t>
+  </si>
+  <si>
+    <t>Le niveau du sol fini se situra à + 0.17m /  niveau haut sol actuel</t>
+  </si>
+  <si>
+    <t>Répartition des tâches :</t>
+  </si>
+  <si>
+    <t>Elec 2M : Bâtiment les Sources + Eclairage Extérieurs + Détection incendie pour les bâtiments Tavaillon et Epilobe</t>
+  </si>
+  <si>
+    <t>Vincentz : Bâtiment le Tavaillon + Epilobe (hors DI) + alimentation générale</t>
+  </si>
+  <si>
+    <t>Les besoins électriques de l'ascensoriste vous ont été transmis ce jour.</t>
+  </si>
+  <si>
+    <t>Vu sur place, tracé modifié du sol fini pour "contourner la fenêtre" sur la façade est</t>
+  </si>
+  <si>
+    <t>Les sous faces de toiture seront laissées en l'état</t>
+  </si>
+  <si>
+    <t>Au RDC bas, une trappe devra être ménagée pour accéder aux tampons de dégorgements des évacuations (dans le local ménage)</t>
+  </si>
+  <si>
+    <t>Au RDC bas, la faïence murale n'est prévue que pour les WC</t>
+  </si>
+  <si>
+    <t>Dans votre situation du mois de Juin, vous pouvez intégrer de la fourniture pour les faïences du bâtiment La Source</t>
+  </si>
+  <si>
+    <t>Nous vous confirmons que les lave-mains dans les WC soivent être installés : ils sont à votre marché</t>
+  </si>
+  <si>
+    <t>Dans le hall, le faux plafond sera aligné avec le haut de la menuiserie. Prendre vos disposition pour connecter avec l'arrivée d'eau.</t>
+  </si>
+  <si>
+    <t>Le réseau de chaleur doit être enfoui à 1.10m sous la surface</t>
+  </si>
+  <si>
+    <t>Teintes et tôlerie identiques à La Source pour la maison du gardien</t>
+  </si>
+  <si>
+    <t>La porte de la chaufferie doit être prévue</t>
+  </si>
+  <si>
+    <t>Confirmation : les 4 fenêtres de toît de La maison du gardien sont à remplacer</t>
+  </si>
+  <si>
+    <t>TS proposés pour Million : réalisation d'un mur à ossature bois sur les pignons de l'Epilobe, car à la démolition ceux-ci se sont avérés pourris - Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposés pour Million : renforts de charpente de l'Epilobe - Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposés pour Million : bardage pignons en lieu et place de l'amiante déposée par Baruch - Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposés pour Million : frein vapeur La Source environ 300 m$^2$ - Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposés pour Grunenwald : calage ITE façade Sud La Source- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposés pour Marion Bois Construction : Ouate de cellulose dans pignon Epilobe + ouate de cellulose dans logement Nord de l'Epilobe, au plafond- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposés Stamile : carrelage dans le couloir La Source- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Moins value proposé Geistel : supression de faux plafonds démontables dans La Source- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Balance financière à réaliser par Leader Platrerie : ajout de faux Plafonds non démontables + reprise de murs abîmés + modification de plans + doublage Nord RDC bas- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Moins value proposée à Hertzog : suppression de sol souple dans le couloir de La Source (remplacé par le carrelage de Stamile)- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Moins value proposée à Million + Nicolas R : pas de réfection de la toîture de la maison du gardien.- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposés : projection d'isolants dans le vide sanitaire de la maison du gardien- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposé Parolini : drainage plateforme Tavaillon- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposé Parolini : remblayage et compactage fosses découvertes sous Le Tavaillon- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposé Parolini : déblaiement du réservoir d'adduction d'eau pour découvrir le trop plein colmaté.- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposé Parolini : raccordement direct dans la chambre de vanne du réservoir- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Moins value proposée Alfa Fenorm : suppression de 8 fenêtres au Nord de La Source- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Plus Value proposée Bari : maçonnerie pour boucher les fenêtres qui ne seront pas mise en place par Alfa Fenorm- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Plus Value proposée Geistel : faux plafond démontable supplémentaire suite à la démolition obligatoire de faux plafond existant dans les ateliers de La Source- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Plus Value proposée Bari : démolition de faux plafond existant dans La Source (il n'était pas possible de les démolir partiellement)- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposé à Parolini : regard dans la chaufferie pour raccordement du réseau de chaleur- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>TS proposé à Parolini : mise en place de 3 regards de tirage sur la tranchée latérale parcourant tout le site + raccordement réseaux d'adduction vers l'auberge + raccordement réseaux d'adduction vers les Coprins- Demande d'accord de principe en vu de proposer un avenant</t>
+  </si>
+  <si>
+    <t>Poursuivre la mise en  \oe uvre des structures de faux plafonds dans les étages, vous rapprocher du lot chauffage ventilation pour bien gérer l'altimétrie de votre structure</t>
+  </si>
+  <si>
+    <t>remplacement dalle de gouttière de la Source, façade Sud uniquement</t>
+  </si>
+  <si>
+    <t>Renforcer l'ancrage de la structure métallique à l'aide de tige fileté + scellement chimique : actuellement, c'est le lamellé collé qui tient la structure métallique !</t>
+  </si>
+  <si>
+    <t>Faire en sorte que votre départ en congé ne bloque pas les autres corps d'état</t>
+  </si>
+  <si>
+    <t>nettoyage du chantier : attention à ne pas jeter les chutes du plaquistes dont il se sert !</t>
+  </si>
+  <si>
+    <t>baro</t>
+  </si>
+  <si>
+    <t>finitions de démolitioins : bosses sur le sol, grater les projections de béton de la cage d'ascenceur sur murs joint, réseaux de VMC</t>
+  </si>
+  <si>
+    <t>finir la dépose de l'ancien appareillage électrique et des anciens câbles</t>
+  </si>
+  <si>
+    <t>Se positionner sur la nécessité d'encoffrer les poutres métalliques de La Source</t>
+  </si>
+  <si>
+    <t>Transmettre votre RIB à la MOA</t>
+  </si>
+  <si>
+    <t>Les entreprises n'ont pas été payées ce mois ci, faire le nécessaire</t>
+  </si>
+  <si>
+    <t>Mettre en place les registres manuels de régalage, en tête de réseaux, comme prévu au marché</t>
+  </si>
+  <si>
+    <t>la mise en place d'une retombé de 5 cm devant l'escalier Est est confirmé (pour jonction avec faux plfond incliné)</t>
+  </si>
+  <si>
+    <t>Le faux plafond incliné entre le faux plafond aléatoire et l'escalier sera réalisé en plâtre lisse</t>
+  </si>
+  <si>
+    <t>Une bande de plâtre lisse de 10 cm pourra être réalisée autour des faux plafond aléatoire (entrée et salle de thérapie)</t>
+  </si>
+  <si>
+    <t>Faut-il réaliser les percements et pénétrations de réseau dans le tavaillon avant la réalisation de l'étanchéité sur les murs enterrés du bâtiment ? Réponse attendue pour le 22/07/2015</t>
+  </si>
+  <si>
+    <t>contrôler l'altimétrie de la poutre lamellé collé par rapport au brut de la dalle coulée par Bari</t>
+  </si>
+  <si>
+    <t>Le regard à mettre en place pour réseau de chaleur dans la chaufferie mesurera 600x600</t>
+  </si>
+  <si>
+    <t>Vous positionner sur l'opportunité de raccorder le réseau de chaleur aux Coprins (éventuellement en conservant le secours gaz ?)</t>
+  </si>
+  <si>
+    <t>Déplacer vos contrepoids pour permettre le déplacement de l'échaffaudage</t>
+  </si>
+  <si>
+    <t>Nettoyer vos déchets situés en base de l'échaffaudage pour permettre son déplacement</t>
+  </si>
+  <si>
+    <t>transmission d'un devis par Parolini pour réfection du réseau d'évacuation de l'Epilobe et raccordement sur le drain du Tavaillon</t>
+  </si>
+  <si>
+    <t>compléter canevas courant faible préparer par le BE Projelec</t>
+  </si>
+  <si>
+    <t>SOUSSECTION</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t>INDICE</t>
+  </si>
+  <si>
     <t>DATE</t>
-  </si>
-  <si>
-    <t>ECHEANCE</t>
-  </si>
-  <si>
-    <t>DATEREALISATION</t>
-  </si>
-  <si>
-    <t>PRIORITE</t>
-  </si>
-  <si>
-    <t>ETAT</t>
-  </si>
-  <si>
-    <t>SECTION</t>
-  </si>
-  <si>
-    <t>ACTEUR</t>
-  </si>
-  <si>
-    <t>TACHE</t>
-  </si>
-  <si>
-    <t>URGENT</t>
-  </si>
-  <si>
-    <t>epb</t>
-  </si>
-  <si>
-    <t>alf</t>
-  </si>
-  <si>
-    <t>Teinte menuiserie à proposer - gris ardoise / gris anthracite. Proposer une tôlerie assortie à l'architecte</t>
-  </si>
-  <si>
-    <t>src</t>
-  </si>
-  <si>
-    <t>Débuter votre intervention par la pose des menuiseries du 1er niveau façade Nord pour permettre une sécurisation de l'accès</t>
-  </si>
-  <si>
-    <t>Dernier délais pour pose des tablettes + menuiseries sud car le lot ITE ainsi que le second \oe uvre du RDC sont bloqués depuis trop longtemps</t>
-  </si>
-  <si>
-    <t>barigo</t>
-  </si>
-  <si>
-    <t>Poursuivre les travaux de terrassement dans la chaufferie + mise en place des réseaux enterrés (compris fourreaux réseau de chaleur en 250 + regard réseau de chaleur + réaliser réseau évacuation dans l'extension des sanitaires.</t>
-  </si>
-  <si>
-    <t>Réaliser le GO de la chaufferie e le GO de  l'extension des sanitaires</t>
-  </si>
-  <si>
-    <t>Etayer pilier Sud-Ouest en amont de la démolition du pignon</t>
-  </si>
-  <si>
-    <t>La réalisation du cuvelage (étanchéité) de la fosse d'ascenseur est à votre lot</t>
-  </si>
-  <si>
-    <t>Intervention de l'ascensoriste prévue à partir du 15 Juillet. Le cuvelage de la fosse doit impérativement être terminé à cette date pour permettre à ce dernier de travailler</t>
-  </si>
-  <si>
-    <t>La chape de La Source va être poncer le 09 Juillet. Débarasser le RDC pour permettre son intervention</t>
-  </si>
-  <si>
-    <t>tav</t>
-  </si>
-  <si>
-    <t>Prévoir intervention sur la maison du gardien pour découper la casquette existante.</t>
-  </si>
-  <si>
-    <t>orga</t>
-  </si>
-  <si>
-    <t>belc</t>
-  </si>
-  <si>
-    <t>Faire un récap sous forme de canevas des prestations prévues au titre des courants faibles sur le site</t>
-  </si>
-  <si>
-    <t>best</t>
-  </si>
-  <si>
-    <t>Suite à la réception du plan EXE R+2 Tavaillon, poursuivre vos études</t>
-  </si>
-  <si>
-    <t>Suite à la réception du plan EXE R+3 Tavaillon, poursuivre vos études</t>
-  </si>
-  <si>
-    <t>Il semblerait que les plans transmis à Bari pour la chaufferie ne contiennent pas les réservations transmises par le lot CVC. Mettre à jour.</t>
-  </si>
-  <si>
-    <t>beth</t>
-  </si>
-  <si>
-    <t>Suite à la réunion du technique du 18 Juin, diffuser le nouveau schéma hydraulique.</t>
-  </si>
-  <si>
-    <t>chi</t>
-  </si>
-  <si>
-    <t>Travaux hors marché : surélever de 10cm la porte provisoire située à l'ouest du bâtiment au RDC bas, la porte qui barre l'accès aux étages</t>
-  </si>
-  <si>
-    <t>Pose des menuiseries intérieures</t>
-  </si>
-  <si>
-    <t>ecp</t>
-  </si>
-  <si>
-    <t>Démontage échaffaudage sur 7 travées à prévoir pour Mercredi 15/07.</t>
-  </si>
-  <si>
-    <t>el2</t>
-  </si>
-  <si>
-    <t>Déplacement des espaces d'attente sécurisés selon plans à paraître semaine prochaine. Prendre dispositions en conséquence.</t>
-  </si>
-  <si>
-    <t>moe</t>
-  </si>
-  <si>
-    <t>Transmettre côte pour baie perpendiculaire à l'escalier au R+1 les Sources</t>
-  </si>
-  <si>
-    <t>L'échaffaudage étant installé, prévoir la dépose du paratonerre.</t>
-  </si>
-  <si>
-    <t>La chape de La Source va être poncer le 09 Juillet. Débarasser le RDC bas pour permettre son intervention</t>
-  </si>
-  <si>
-    <t>Prévoir intervention sur la maison du gardien pour les modifications en façade (coffret force / lumière)</t>
-  </si>
-  <si>
-    <t>grw</t>
-  </si>
-  <si>
-    <t>L'isolation du RDC de l'Epilobe, depuis l'extérieur (dans les locaux condamnés) peut être prévue. Epaisseur à prévoir : 12 cm de polystyrène, isolation des murs et des plafonds</t>
-  </si>
-  <si>
-    <t>Intervenir pour mettre en place isolant entre menuiseries et avant toît au R+1 avant le démontage de l'échaffaudage jusqu'à la finition extérieure</t>
-  </si>
-  <si>
-    <t>Terminer enduit au dessus des menuiseries des travées centrales pour le Mercredi 15/07, date de démontage de l'échaffaudage</t>
-  </si>
-  <si>
-    <t>Donner emplacement bouche incendie à Parolini</t>
-  </si>
-  <si>
-    <t>gst</t>
-  </si>
-  <si>
-    <t>Intervention pour réalisation des plafonds démontables. Commencer par RDC Haut et R+1 salle situées au Sud - attendre intervention de l'électricien pour intervention dans les circulations Nord  des niveaux supérieurs et le RDC Bas</t>
-  </si>
-  <si>
-    <t>htz</t>
-  </si>
-  <si>
-    <t>La chape de La Source va être poncer le 09 Juillet. Débarasser le RDC bas pour permettre son intervention + programmer intervention à la suite</t>
-  </si>
-  <si>
-    <t>RAPPEL</t>
-  </si>
-  <si>
-    <t>Vous rapprocher de M Million pour organiser la livraison de la paille</t>
-  </si>
-  <si>
-    <t>laem</t>
-  </si>
-  <si>
-    <t>Intervention serrurerie pour pergolas</t>
-  </si>
-  <si>
-    <t>Programmer découpe partielle de l'escalier métallique existant sur la maison du gardien.</t>
-  </si>
-  <si>
-    <t>ldr</t>
-  </si>
-  <si>
-    <t>L'espace compris entre la volée ascendante de marche et la cloison construite dans l'escalier doit être colmatter par une "mini paillasse" en plâtre qui supportera du carelage</t>
-  </si>
-  <si>
-    <t>Travaux complémentaires plâtrerie, conformément aux crobarres transmis</t>
-  </si>
-  <si>
-    <t>Boucher les trous au plâtre pour permettre l'intervention de Gaistel</t>
-  </si>
-  <si>
-    <t>Mise en place doublage dans les cages d'escalier</t>
-  </si>
-  <si>
-    <t>Attention : vous êtes en retard sur les enduites de rebouchage de trous, le faux plafond démontable attend après vous</t>
-  </si>
-  <si>
-    <t>Vu sur site : encoffrer poutre métalique au RDC bas</t>
-  </si>
-  <si>
-    <t>mcb</t>
-  </si>
-  <si>
-    <t>Transmettre devis pour insufflation supplémentaire + frein-vapeur + contre-lattage sur 57 m$^2$ / épaisseur 13 cm dans l'Epilobe</t>
-  </si>
-  <si>
-    <t>Prévoir intervention pour soufflage ouate dans plancher bas R+2 à partir du 25 Mai - Reporté 08/06/2015</t>
-  </si>
-  <si>
-    <t>mil</t>
-  </si>
-  <si>
-    <t>Travaux sur MOB chaufferie à partir du 10 Aout 2015</t>
-  </si>
-  <si>
-    <t>Intervention sur la façade des sources pour mise en place bardage + casquettes brise soleil à partir du 22/07/2015</t>
-  </si>
-  <si>
-    <t>moa</t>
-  </si>
-  <si>
-    <t>Participer à la réunion du 27 Mars 14h00 pour finaliser l'appareillage électrique dans l'Epilobe</t>
-  </si>
-  <si>
-    <t>La réunion du 22 avec M Weulersse est déplacée à 15h</t>
-  </si>
-  <si>
-    <t>Fournir puissance électrique pour raccordement Auberge + Caprin</t>
-  </si>
-  <si>
-    <t>Terminer balance financière pour Parolini</t>
-  </si>
-  <si>
-    <t>Programmer test d'étanchéité à l'air + étanchéité à l'air des réseaux</t>
-  </si>
-  <si>
-    <t>Préciser architecture France Telecom + adduction d'eau bâtiment Epilobe.</t>
-  </si>
-  <si>
-    <t>Redessiner le réseau de chaleur</t>
-  </si>
-  <si>
-    <t>Une balance financière a été proposée par l'entreprise Million. Donner un avis et transmettre une proposition d'avenant à la Maîtrise d'Ouvrage</t>
-  </si>
-  <si>
-    <t>Reprendre le planning en intégrant les congés pour transmettre dates d'intervention à Million + transmettre planning OPC à la MOA</t>
-  </si>
-  <si>
-    <t>Mettre à jour plan réseau de chaleur</t>
-  </si>
-  <si>
-    <t>Transmettre plans à Chiodetti pour l'Epilobe (réservations)</t>
-  </si>
-  <si>
-    <t>Proposer un canevas pour fonctionnement Courants Faibles sur l'ensemble du site</t>
-  </si>
-  <si>
-    <t>Transmettre côtes de la limite préau sur la façade est pour que l'ITE puisse s'arrêter au bon endroit.</t>
-  </si>
-  <si>
-    <t>Réaliser un état des lieux général du chantier du point de vue financier intégrant toutes plus values / moins values connues à ce jour.</t>
-  </si>
-  <si>
-    <t>Préparer OS GO pour signature par le MOA</t>
-  </si>
-  <si>
-    <t>Contacter Eric Michel, chef des pompiers à Orbey, pour valider le principe de "réserve incendie"</t>
-  </si>
-  <si>
-    <t>La réunion du 22 avec M Barth et M Bourcard est déplacée à 15h</t>
-  </si>
-  <si>
-    <t>nic</t>
-  </si>
-  <si>
-    <t>Boucher les cheminées + mettre en place les fenêtre de toîts + déplacer la dalle de gouttière</t>
-  </si>
-  <si>
-    <t>Commander fenêtres de toît en triple vitrage</t>
-  </si>
-  <si>
-    <t>remplacement dalle de gouttière de la Source, façade Nord et Sud</t>
-  </si>
-  <si>
-    <t>Réaliser l'étanchéité des murs enterrés du RDC au Nord du Tavaillon</t>
-  </si>
-  <si>
-    <t>paro</t>
-  </si>
-  <si>
-    <t>Prévoir évacuations sous la boulangerie à partir du 18 Mai</t>
-  </si>
-  <si>
-    <t>Prévoir raccordement avaloir de la réserve situé au Nord niveau 0 de l'Epilobe vers le collecteur EU situé sous les WC.</t>
-  </si>
-  <si>
-    <t>Terrassement à prévoir sous la chaufferie à partir du 01 Juillet.</t>
-  </si>
-  <si>
-    <t>Devis à transmettre pour : travaux en supplément dans la chaufferie pour installation d'un regard + fourreaux pour raccordement du réseau de chaleur</t>
-  </si>
-  <si>
-    <t>Programmer de tirer une évacuation pour raccordement au réseau EU depuis sous-station SOURCE</t>
-  </si>
-  <si>
-    <t>Une canalisation d'eau a été endommagée, elle déverse sur l'échaffaudage ce qui ravine ses fondation. La manchonner en urgence pour que cessent les dégâts</t>
-  </si>
-  <si>
-    <t>Transmettre Bon de Livraisons pour justifier différence entre le calcul de l'architecte et vos mêtrés pour les travaux en plus value</t>
-  </si>
-  <si>
-    <t>phb</t>
-  </si>
-  <si>
-    <t>Transmettre les éléments de réservations manquant actuellement à ceux précédemment transmis : mur Est de la chaufferie contre bâtiment existant, VB, VH -  revoir emplacement cheminée.</t>
-  </si>
-  <si>
-    <t>Transmettre les réservations dans les parois de la chaufferie à Gettec, compris les réservations du mur Est de la chaufferie ainsi que la VB et la VH</t>
-  </si>
-  <si>
-    <t>Dès que la mise à jour des plans sera réalisée par l'architecte, prévoir de mettre en place les tubes d'alimentation chauffage pour les radiateurs R+2 de l'Epilobe</t>
-  </si>
-  <si>
-    <t>Prévoir commande CTA pour pose fin Mai</t>
-  </si>
-  <si>
-    <t>Programmer test étanchéité à l'air du réseau à la suite de votre intervention pour le 03 Juin</t>
-  </si>
-  <si>
-    <t>L'étanchéité à l'air des réseaux devra être renforcée : joint des gaines + mastic + ruban adhésif pour atteindre une classe d'étanchéité des réseaux correcte</t>
-  </si>
-  <si>
-    <t>Réaliser calfeutrement propre au plâtre pour réencoffrage des IPN.</t>
-  </si>
-  <si>
-    <t>Prévoir la mise en place de grilles prise d'air / rejet d'air sur le pignon Ouest du bâtiment + chiffrer la mise en place de grilles pour ventilation du comble perdus. Intervention urgente pour permettre au lot ITE de poursuivre.</t>
-  </si>
-  <si>
-    <t>Le plenum de la salle thérapie mesure 4 cm. Il est nécessaire de repasser les gaines dans la circulation.</t>
-  </si>
-  <si>
-    <t>Les registres d'équilibrage dans le réseau de La Source n'ont pas été mis en place. Prévoir leur mise en place.</t>
-  </si>
-  <si>
-    <t>Laquez les grilles extérieures en blanc selon RAL 9001</t>
-  </si>
-  <si>
-    <t>Transmettre réservations dans les Prémurs pour synthèse</t>
-  </si>
-  <si>
-    <t>Transmettre réservation dans R+2 suite à la diffusion des plans ARCHI EXE</t>
-  </si>
-  <si>
-    <t>Lors de votre intervention pour dépose et évacuation des chaudières de La Source et de L'Epilobe, vos équipes ont disqué des poteaux servant d'étendoir à linge hors de toute demande de la part de la maîtrise d'\oe uvre, à la suite de quoi des éléments métalliques émergents sont demeurés sur site, camouflés par la pelouse. Cette semaine, la société BARI a vu l'un de ses engins malheureusement creuver sur l'une de ces émergences. Constaté ce jour sur site 15/04/2015. Merci de vous rapprocher de la société BARI afin de trouver une solution à l'amiable à cet incident.</t>
-  </si>
-  <si>
-    <t>Transmettre réservation dans le R+3 suite à la diffusion des plans ARCHI EXE</t>
-  </si>
-  <si>
-    <t>URGENT : vous rapprocher de Bari pour intégrer ce qu'il faut dans les prémurs (alimentation radiateurs). Les prémurs sont en train d'être mis en place !</t>
-  </si>
-  <si>
-    <t>Dans la chaufferie, prévoir un raccordement dans un regard pour le réseau de chaleur</t>
-  </si>
-  <si>
-    <t>Programmer interventions pour réseau en dalle haute RDC pour le 13 Juillet 2015</t>
-  </si>
-  <si>
-    <t>sch</t>
-  </si>
-  <si>
-    <t>Les sujétions à votre installations concernant la tige fileté sur le mur Est de la cage d'ascenseur sont à votre charge. Si vous souhaitez sous-traite votre intervention à la société Bari, les contacter pour leur donner les instructions.</t>
-  </si>
-  <si>
-    <t>stm</t>
-  </si>
-  <si>
-    <t>tch</t>
-  </si>
-  <si>
-    <t>Ponçage de la chape programmé pour le 09/07/2015 - récupérer clé d'accès au chantier auprès de Nicolas Bourcard</t>
-  </si>
-  <si>
-    <t>ths</t>
-  </si>
-  <si>
-    <t>Mise en place réseaux + évacuations des logements R+2 Epilobe selon plans architectes transmis le 07/07/2015</t>
-  </si>
-  <si>
-    <t>vcz</t>
-  </si>
-  <si>
-    <t>Réaliser dossier administratif « demande de raccordement »</t>
-  </si>
-  <si>
-    <t>Finaliser la demande de raccordement ERDF</t>
-  </si>
-  <si>
-    <t>Le 23 Mars 2015, l'architecte va donner les instructions côtées au lot démolition sur site, notamment en relation avec le passage des réseaux. Transmettre éléments complémentaires au dossier Marché si  besoin</t>
-  </si>
-  <si>
-    <t>Diffusion plan de réservation Epilobe pour le 22/04/2015</t>
-  </si>
-  <si>
-    <t>Prévoir terrassement pour chaufferie à partir du 05/05/2015</t>
-  </si>
-  <si>
-    <t>Prévoir 1er intervention à partir du 18 Mai pour évacuation et alimentation des logements R+2 situés à l'intérieur du plancher en cours de construction</t>
-  </si>
-  <si>
-    <t>Intervention à prévoir à partir du 27 Mai - Reporté 03 Juin</t>
-  </si>
-  <si>
-    <t>Programmer interventions nécessaires en réseaux enterrés sous la chaufferie conjointement au travail du lot terrassement pour la semaine du 06 Juillet.</t>
-  </si>
-  <si>
-    <t>Prévoir jambe de force pour soutien des pannes</t>
-  </si>
-  <si>
-    <t>Prévoir de rehausser les pannes + faîtage</t>
-  </si>
-  <si>
-    <t>Programmer intervention pour réalisation de l'étanchéité contre les murs enterrés à partir du  13 Juillet 2015</t>
-  </si>
-  <si>
-    <t>et de l'Epilobe pour permettre à Bari de poursuivre son travail.</t>
-  </si>
-  <si>
-    <t>Tracer sur site les réservations dans l'Epilobe + La Source - RDV pris avec Bari</t>
-  </si>
-  <si>
-    <t>CHAUFFERIE : transmettre réservations à GETTEC</t>
-  </si>
-  <si>
-    <t>TS proposés pour Grunenwald : peinture sous face avant toît La Source- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Intervention à programmer pour réaliser les structure pare soleil de la façade pour mi-avril Début Mai.</t>
-  </si>
-  <si>
-    <t>Alimentation des radiateurs des circulations en apparents comme proposé validée</t>
-  </si>
-  <si>
-    <t>Sur 7 travées, l'échaffaudage devra être déplacé afin de se retrouver à 80 cm du mur. Aux abouts des travées restant "proche" de la façade, des équerres devront être fournies pour permettre au lot ITE de travailler (finitions sur casquettes bakélite). Votre intervention ne pourra se faire avant le 06 Juillet, car l'ITE doit, au préalable poser un isolant au dessus des menuiseries R+1 (sous l'avant toît qui deviendra inaccessible une fois les casquettes bakélites posées). Transmettre devis Travaux Supplémentaires.</t>
-  </si>
-  <si>
-    <t>Raccorder chauffe eau (celui en face à gauche dans la chaufferie) pour production ECS - attente eau</t>
-  </si>
-  <si>
-    <t>Vous coordoner avec Herrbach pour mettre en place le réseau de chaleur.</t>
-  </si>
-  <si>
-    <t>L'alimentation en eau de l'Epilobe se fera via la chaufferie et en tranchée commune avec le réseau de chaleur.</t>
-  </si>
-  <si>
-    <t>TS proposé à Herrbach : mise en place d'une liaison en réseau de chaleur entre l'auberge et Le Tavaillon- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Moins value proposée Parolini : suppression du réseau d'adduction spécifique incendie, vu avec le SDIS- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>transmission d'un devis par ECP pour lui permettre de démonter / remonter les 7 travées centrales d'échaffaudage au Sud, pour la mise en place des casquettes brise soleil.</t>
-  </si>
-  <si>
-    <t>transmission d'un devis par Nicolas R pour remplacement des dalles de gouttière du bâtiment la source</t>
-  </si>
-  <si>
-    <t>baridem</t>
-  </si>
-  <si>
-    <t>Ouverture tranchée pour évacuations RDC</t>
-  </si>
-  <si>
-    <t>Réalisation des travaux sur la boulangerie à partir 01 Juin 2015</t>
-  </si>
-  <si>
-    <t>Prévoir le renforcement de la fixation du portique métallique (actuellement fixé sur un lintaux qui va être détruit)</t>
-  </si>
-  <si>
-    <t>Finaliser votre intervention en liant la structure métallique à la façade. Le maçon attend après vous.</t>
-  </si>
-  <si>
-    <t>Fournir éléments complémentaires désenfumage</t>
-  </si>
-  <si>
-    <t>Donnez vos prescriptions pour améliorer l'étanchéité à l'air du système de désenfumage</t>
-  </si>
-  <si>
-    <t>Terminer balance financière pour Million</t>
-  </si>
-  <si>
-    <t>SOURCE : faire le point sur les poignées de portes intérieures / serrures moletées</t>
-  </si>
-  <si>
-    <t>Aboutir à une solution accepté par FIBE et le BCT pour les clapets d'étanchéité à l'air dans les gaines de désenfumage du Tavaillon</t>
-  </si>
-  <si>
-    <t>Validation du raccordement en 160 sur la conduite existante de diamètre 90 intérieur</t>
-  </si>
-  <si>
-    <t>Choisir teinte enduit de finition La Source - Urgent pour permettre au lot ITE de travailler.</t>
-  </si>
-  <si>
-    <t>Transmettre à Parolini : plans réseaux sous chaufferie, drains, plan chaufferie, plan GO</t>
-  </si>
-  <si>
-    <t>Vous rapprocher de Thomas Weulersse pour étudier une alternative en Zinc sur la maison du Gardien.</t>
-  </si>
-  <si>
-    <t>Le vide sanitaire de la maison du gardien est isolé par 3 cm de polystyrène. Vérifier que cela permette d'atteindre les exigences de la labellisation (en conservant également la toiture existante).</t>
-  </si>
-  <si>
-    <t>EPILOBE : Transmettre plans EXE à Theisen</t>
-  </si>
-  <si>
-    <t>Evacuer radiateurs vers ferrailleur comme vu sur site</t>
-  </si>
-  <si>
-    <t>Contacter France Telecom pour qu'ils nous communiquent leurs arrivées sur le site</t>
-  </si>
-  <si>
-    <t>Transmettre diamètres raccordement AEP à Parolini</t>
-  </si>
-  <si>
-    <t>Mettre à jour le plan des réseaux pour l'ensemble du site et le transmettre à Parolini et Muré</t>
-  </si>
-  <si>
-    <t>Déterminer avec Thomas le principe d'évacuation des EP du bâtiment - notamment, vérifier que le tube Coupé à l'Est du bâtiment n'est pas relié à la descente à l'angle Nord Est</t>
-  </si>
-  <si>
-    <t>Programmer l'intervention sur le bâtiment La Source pour le mois de Mai</t>
-  </si>
-  <si>
-    <t>Reprendre feuillures portes d'entrée du RDC haut</t>
-  </si>
-  <si>
-    <t>Travaux hors marché : fourniture et pose de 3 cylindres pour les portes provisoires</t>
-  </si>
-  <si>
-    <t>Lors de votre intervention, stocker proprement les garde-corps intérieurs de l'échaffaudage</t>
-  </si>
-  <si>
-    <t>Les tubes associés aux emplacements de radiateurs initiaux doivent être supprimer et bouchonnés.</t>
-  </si>
-  <si>
-    <t>Poursuivre votre intervention dans le bâtiment</t>
-  </si>
-  <si>
-    <t>Réaliser en priorité les travaux dans le WC du RDC bas pour permettre au carreleur de travailler</t>
-  </si>
-  <si>
-    <t>Réaliser une cloison provisoire au RDC bas, à droite de l'ascenseur pour sécuriser l'accès aux étages vis-à-vis du vol</t>
-  </si>
-  <si>
-    <t>Prioriser votre intervention sur les WC de l'ensemble des niveaux pour permettre au carreleur de travailler</t>
-  </si>
-  <si>
-    <t>1.5 cm à rattraper entre les menuiseries à l'est et celle au sud en mordant sur le chassis fixe situé à l'Est</t>
-  </si>
-  <si>
-    <t>L'échaffaudage va être démonter sur les 7 travées centrales, coordonner votre intervention pour mise en place de la pergola.</t>
-  </si>
-  <si>
-    <t>Programmer intervention pour ponçage de la chape</t>
-  </si>
-  <si>
-    <t>Réalisation cloisons provisoires au RDC bas et au RDC haut pour permettre la sécurisation du site - nota au RDC Bas, la cloison doit laisser un espace de 15 cm sous le plâtre pour permettre au carreleur de travailler</t>
-  </si>
-  <si>
-    <t>Remplacer chassis désenfumage R+1 par chassis fixe</t>
-  </si>
-  <si>
-    <t>Pour les menuiseries non posées (portes d'entrées Source) , poser l'isolant jusqu'à une distance de 50 cm de la menuiserie</t>
-  </si>
-  <si>
-    <t>Le rejet d'air a finalement été déplacé au RDC bas centré sur la fenêtre pour respecter une distance optimisée entre prise et rejet.</t>
-  </si>
-  <si>
-    <t>Confirmation : les réservations dans les cloisonnements intérieurs sont à votre charge.</t>
-  </si>
-  <si>
-    <t>Commander l'ascenseur pour pose à partir du 25/05/2015</t>
-  </si>
-  <si>
-    <t>Commander ascenceur pour pose à la mi Juin</t>
-  </si>
-  <si>
-    <t>Votre intervention peut débuter dans les étages.</t>
-  </si>
-  <si>
-    <t>L'eau chaude alimentant le lavoir devra être isolée.</t>
-  </si>
-  <si>
-    <t>Mettre en place les clôtures de chantier selon le PGC.</t>
-  </si>
-  <si>
-    <t>Transmettre réservation dans R+2</t>
-  </si>
-  <si>
-    <t>Réalisation des fondations</t>
-  </si>
-  <si>
-    <t>URGENT : vous rapprocher de Bari pour intégrer ce qu'il faut dans les prémurs (évacuations et éventuellement alimentation). Les prémurs sont en train d'être mis en place !</t>
-  </si>
-  <si>
-    <t>Le réseau de chaleur n'empruntant pas le même cheminement, réaliser le fanchissement du parking pour l'alimentation EF uniquement.</t>
-  </si>
-  <si>
-    <t>Poursuivre les travaux selon planning. Transmettre votre période de congé.</t>
-  </si>
-  <si>
-    <t>Transmettre dès réceptions des plans des prémurs vos incorporations</t>
-  </si>
-  <si>
-    <t>Prévoir intervention si vous avez des incorporations dans la dalle basse RDC dès la semaine prochaine</t>
-  </si>
-  <si>
-    <t>Les seuils des portes en granit doivent faire une hauteur de 7 cm.</t>
-  </si>
-  <si>
-    <t>5 menuiseries R+2 sur pignons Est et Ouest seront posées en applique intérieure</t>
-  </si>
-  <si>
-    <t>La double porte et la simple porte sur la façade sud sont inversées</t>
-  </si>
-  <si>
-    <t>Les fenêtres fixes sur les plans (R+1 Sud) sont effectivement fixes</t>
-  </si>
-  <si>
-    <t>Les fenêtres qui ne sont pas à votre marché (R+2) ne seront pas réalisées</t>
-  </si>
-  <si>
-    <t>La nouvelle fenêtre à l'Est RDC sera de type 2 OB - 1er ouvrant à gauche vu de  l'intérieur</t>
-  </si>
-  <si>
-    <t>La fenêtre situé au RDC à l'est sur le mur restant à construire sera de type pose en applique</t>
-  </si>
-  <si>
-    <t>Le bardage choisie est de type rainuré languette, largeur des lames : 18 cm (cf. photo en fin de compte-rendu)</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>Interdiction d'accéder aux armoires électriques situées dans La Source : elles sont sous tension.</t>
-  </si>
-  <si>
-    <t>Seules les entreprises habilitées peuvent intervenir sur l'amiante, Interdiction notamment à toute entreprise non habilitée d'intervenir sur la couverture du bâtiment Epilobe</t>
-  </si>
-  <si>
-    <t>Des clés de la base-vie sont disponible auprès de M Dulau - se manifester</t>
-  </si>
-  <si>
-    <t>1 seule situation mensuelle est accepté, elle doit être transmise dernière semaine du mois pour validation lors de la première semaine du mois suivant</t>
-  </si>
-  <si>
-    <t>Le port du casque est obligatoire sur l'ensemble du chantier</t>
-  </si>
-  <si>
-    <t>Désormais, les factures transmises après la dernière semaine du mois ne seront traitées qu'à la fin du mois suivant par la maîtrise d'\oe uvre</t>
-  </si>
-  <si>
-    <t>Le RDC haut et le R+1 de La Source sont désormais condamnés. Des clés sont disponibles auprès de M Bourcard. Il est impératif de refermer le chantier chaque soir.</t>
-  </si>
-  <si>
-    <t>Le chemin sera coupé pendant 3 semaine au niveau des travaux de terrassement en chaufferie à partir du 15 Juillet</t>
-  </si>
-  <si>
-    <t>Plan EXE La Source : l'arrivée d'eau du bâtiment Source se fera dans le local sous station sous l'escalier</t>
-  </si>
-  <si>
-    <t>Etudier le détail d'alimentation des BSO au travers de la paille (sécurité ?) - le câble passe derrière le parement intérieur puis traverse la façade au niveau du lintau bois (à percer) au dessus de la fenêtre</t>
-  </si>
-  <si>
-    <t>Etudier le détail de l'alimentation des détecteurs de fumée situés en applique sous les faux plafonds coupe feu -  a priori  système de double plafond au R+3 et dalle brute dans les chambres donc pas de problème</t>
-  </si>
-  <si>
-    <t>Nota : leader platrerie sera en congé à partir du 24 Juillet</t>
-  </si>
-  <si>
-    <t>sps</t>
-  </si>
-  <si>
-    <t>Le poteau situé à proximité du bâtiment Les Caprins sera rapidement hors service et ce pour la durée du chantier</t>
-  </si>
-  <si>
-    <t>Le 04 Avril 2015, M Weulersse vous a notifié par mail le choix du modèle et de la teinte pour la protection solaire : Fundermax 3003 NT Rubinus Red - il est urgent de le mettre en commande - Rappel : l'échaffaudage sera installé durant 2 mois seulement</t>
-  </si>
-  <si>
-    <t>Le bardage doit être également commandé rapidement : bardage en mélèze sans teinte avec fibre verticale - Rappel : l'échaffaudage sera installé durant 2 mois seulement</t>
-  </si>
-  <si>
-    <t>Vous avez proposé une alternative à la solution proposé par Terranergie. Ceux-ci la refuse. Merci de mettre vos plans et vos commandes en cohérence avec les remarques du BET</t>
-  </si>
-  <si>
-    <t>Ventiler également les locaux bureau (soufflage 60 m3/h) + maintenance rangement/ RDC et reprise (60 m3/h)</t>
-  </si>
-  <si>
-    <t>Des plafonds type aléatoires '5/15/20' doivent être posés dans le hall d'entrée et dans la pièce thérapie au R+1</t>
-  </si>
-  <si>
-    <t>Poursuivre votre intervention - les menuiseries intérieures peuvent être posées dans les étages</t>
-  </si>
-  <si>
-    <t>Repose des radiateurs non habillés validé</t>
-  </si>
-  <si>
-    <t>Choix des teintes : peinture sous face avant toît RAL 3009 , crépis RAL 9001</t>
-  </si>
-  <si>
-    <t>Les portes au Nord seront à passage PMR ; le grand ouvrant sera aligner avec le couloir faisant face ; pas de traverse horizontale.</t>
-  </si>
-  <si>
-    <t>Confirmation : Sol fini = sol brut + 0.17m</t>
-  </si>
-  <si>
-    <t>La teinte choisi par la MOE et le MOA pour les menuiseries de la Source est KASTANIE selon nuancier proposé</t>
-  </si>
-  <si>
-    <t>Remettre en place les garde-corps intérieurs de l'échaffaudage à la suite de votre intervention</t>
-  </si>
-  <si>
-    <t>Soigner la mise en \oe uvre des vitrages, au silicone, sur les chassis fixes faite sur chantier. L'expérience montre que cela peut être des faiblesses en terme d'étanchéité à l'air</t>
-  </si>
-  <si>
-    <t>En raison du retard sur votre intervention dans le bâtiment des dispositions ont été prises pour fermer l'accès aux étages du bâtiment La Source.</t>
-  </si>
-  <si>
-    <t>ATTENTION : les revêtements des escaliers seront conservés, les protéger afin qu'ils ne soient pas abîmer par la démolition</t>
-  </si>
-  <si>
-    <t>Le niveau du sol fini se situra à + 0.17m /  niveau haut sol actuel</t>
-  </si>
-  <si>
-    <t>Répartition des tâches :</t>
-  </si>
-  <si>
-    <t>Elec 2M : Bâtiment les Sources + Eclairage Extérieurs + Détection incendie pour les bâtiments Tavaillon et Epilobe</t>
-  </si>
-  <si>
-    <t>Vincentz : Bâtiment le Tavaillon + Epilobe (hors DI) + alimentation générale</t>
-  </si>
-  <si>
-    <t>Les besoins électriques de l'ascensoriste vous ont été transmis ce jour.</t>
-  </si>
-  <si>
-    <t>Vu sur place, tracé modifié du sol fini pour "contourner la fenêtre" sur la façade est</t>
-  </si>
-  <si>
-    <t>Les sous faces de toiture seront laissées en l'état</t>
-  </si>
-  <si>
-    <t>Au RDC bas, une trappe devra être ménagée pour accéder aux tampons de dégorgements des évacuations (dans le local ménage)</t>
-  </si>
-  <si>
-    <t>Au RDC bas, la faïence murale n'est prévue que pour les WC</t>
-  </si>
-  <si>
-    <t>Dans votre situation du mois de Juin, vous pouvez intégrer de la fourniture pour les faïences du bâtiment La Source</t>
-  </si>
-  <si>
-    <t>Nous vous confirmons que les lave-mains dans les WC soivent être installés : ils sont à votre marché</t>
-  </si>
-  <si>
-    <t>Dans le hall, le faux plafond sera aligné avec le haut de la menuiserie. Prendre vos disposition pour connecter avec l'arrivée d'eau.</t>
-  </si>
-  <si>
-    <t>Le réseau de chaleur doit être enfoui à 1.10m sous la surface</t>
-  </si>
-  <si>
-    <t>Teintes et tôlerie identiques à La Source pour la maison du gardien</t>
-  </si>
-  <si>
-    <t>La porte de la chaufferie doit être prévue</t>
-  </si>
-  <si>
-    <t>Confirmation : les 4 fenêtres de toît de La maison du gardien sont à remplacer</t>
-  </si>
-  <si>
-    <t>TS proposés pour Million : réalisation d'un mur à ossature bois sur les pignons de l'Epilobe, car à la démolition ceux-ci se sont avérés pourris - Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposés pour Million : renforts de charpente de l'Epilobe - Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposés pour Million : bardage pignons en lieu et place de l'amiante déposée par Baruch - Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposés pour Million : frein vapeur La Source environ 300 m$^2$ - Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposés pour Grunenwald : calage ITE façade Sud La Source- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposés pour Marion Bois Construction : Ouate de cellulose dans pignon Epilobe + ouate de cellulose dans logement Nord de l'Epilobe, au plafond- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposés Stamile : carrelage dans le couloir La Source- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Moins value proposé Geistel : supression de faux plafonds démontables dans La Source- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Balance financière à réaliser par Leader Platrerie : ajout de faux Plafonds non démontables + reprise de murs abîmés + modification de plans + doublage Nord RDC bas- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Moins value proposée à Hertzog : suppression de sol souple dans le couloir de La Source (remplacé par le carrelage de Stamile)- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Moins value proposée à Million + Nicolas R : pas de réfection de la toîture de la maison du gardien.- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposés : projection d'isolants dans le vide sanitaire de la maison du gardien- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposé Parolini : drainage plateforme Tavaillon- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposé Parolini : remblayage et compactage fosses découvertes sous Le Tavaillon- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposé Parolini : déblaiement du réservoir d'adduction d'eau pour découvrir le trop plein colmaté.- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposé Parolini : raccordement direct dans la chambre de vanne du réservoir- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Moins value proposée Alfa Fenorm : suppression de 8 fenêtres au Nord de La Source- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Plus Value proposée Bari : maçonnerie pour boucher les fenêtres qui ne seront pas mise en place par Alfa Fenorm- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Plus Value proposée Geistel : faux plafond démontable supplémentaire suite à la démolition obligatoire de faux plafond existant dans les ateliers de La Source- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Plus Value proposée Bari : démolition de faux plafond existant dans La Source (il n'était pas possible de les démolir partiellement)- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposé à Parolini : regard dans la chaufferie pour raccordement du réseau de chaleur- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>TS proposé à Parolini : mise en place de 3 regards de tirage sur la tranchée latérale parcourant tout le site + raccordement réseaux d'adduction vers l'auberge + raccordement réseaux d'adduction vers les Coprins- Demande d'accord de principe en vu de proposer un avenant</t>
-  </si>
-  <si>
-    <t>Poursuivre la mise en  \oe uvre des structures de faux plafonds dans les étages, vous rapprocher du lot chauffage ventilation pour bien gérer l'altimétrie de votre structure</t>
-  </si>
-  <si>
-    <t>remplacement dalle de gouttière de la Source, façade Sud uniquement</t>
-  </si>
-  <si>
-    <t>Renforcer l'ancrage de la structure métallique à l'aide de tige fileté + scellement chimique : actuellement, c'est le lamellé collé qui tient la structure métallique !</t>
-  </si>
-  <si>
-    <t>Faire en sorte que votre départ en congé ne bloque pas les autres corps d'état</t>
-  </si>
-  <si>
-    <t>nettoyage du chantier : attention à ne pas jeter les chutes du plaquistes dont il se sert !</t>
-  </si>
-  <si>
-    <t>baro</t>
-  </si>
-  <si>
-    <t>finitions de démolitioins : bosses sur le sol, grater les projections de béton de la cage d'ascenceur sur murs joint, réseaux de VMC</t>
-  </si>
-  <si>
-    <t>finir la dépose de l'ancien appareillage électrique et des anciens câbles</t>
-  </si>
-  <si>
-    <t>Se positionner sur la nécessité d'encoffrer les poutres métalliques de La Source</t>
-  </si>
-  <si>
-    <t>Transmettre votre RIB à la MOA</t>
-  </si>
-  <si>
-    <t>Les entreprises n'ont pas été payées ce mois ci, faire le nécessaire</t>
-  </si>
-  <si>
-    <t>Mettre en place les registres manuels de régalage, en tête de réseaux, comme prévu au marché</t>
-  </si>
-  <si>
-    <t>la mise en place d'une retombé de 5 cm devant l'escalier Est est confirmé (pour jonction avec faux plfond incliné)</t>
-  </si>
-  <si>
-    <t>Le faux plafond incliné entre le faux plafond aléatoire et l'escalier sera réalisé en plâtre lisse</t>
-  </si>
-  <si>
-    <t>Une bande de plâtre lisse de 10 cm pourra être réalisée autour des faux plafond aléatoire (entrée et salle de thérapie)</t>
-  </si>
-  <si>
-    <t>Faut-il réaliser les percements et pénétrations de réseau dans le tavaillon avant la réalisation de l'étanchéité sur les murs enterrés du bâtiment ? Réponse attendue pour le 22/07/2015</t>
-  </si>
-  <si>
-    <t>contrôler l'altimétrie de la poutre lamellé collé par rapport au brut de la dalle coulée par Bari</t>
-  </si>
-  <si>
-    <t>Le regard à mettre en place pour réseau de chaleur dans la chaufferie mesurera 600x600</t>
-  </si>
-  <si>
-    <t>Vous positionner sur l'opportunité de raccorder le réseau de chaleur aux Coprins (éventuellement en conservant le secours gaz ?)</t>
-  </si>
-  <si>
-    <t>Déplacer vos contrepoids pour permettre le déplacement de l'échaffaudage</t>
-  </si>
-  <si>
-    <t>Nettoyer vos déchets situés en base de l'échaffaudage pour permettre son déplacement</t>
-  </si>
-  <si>
-    <t>transmission d'un devis par Parolini pour réfection du réseau d'évacuation de l'Epilobe et raccordement sur le drain du Tavaillon</t>
-  </si>
-  <si>
-    <t>compléter canevas courant faible préparer par le BE Projelec</t>
-  </si>
-  <si>
-    <t>SOUSSECTION</t>
-  </si>
-  <si>
-    <t>PLAN</t>
-  </si>
-  <si>
-    <t>NUM</t>
-  </si>
-  <si>
-    <t>INDICE</t>
   </si>
   <si>
     <t>plans</t>
@@ -2068,7 +2071,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2078,6 +2081,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2104,8 +2111,8 @@
   </sheetPr>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3521,15 +3528,16 @@
   </sheetPr>
   <dimension ref="A1:H251"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7206477732794"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9054,8 +9062,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9063,11 +9071,12 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4251012145749"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7206477732794"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>297</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -9299,7 +9308,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -9319,7 +9328,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -9328,7 +9337,7 @@
       <c r="C13" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F13" s="0" t="s">
@@ -9339,7 +9348,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -9348,7 +9357,7 @@
       <c r="C14" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F14" s="0" t="s">
@@ -9359,7 +9368,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -9368,7 +9377,7 @@
       <c r="C15" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F15" s="0" t="s">
@@ -9379,7 +9388,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -9388,7 +9397,7 @@
       <c r="C16" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="4"/>
       <c r="F16" s="0" t="s">
         <v>267</v>
       </c>
@@ -9397,7 +9406,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -9406,7 +9415,7 @@
       <c r="C17" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="4"/>
       <c r="F17" s="0" t="s">
         <v>267</v>
       </c>
@@ -9415,7 +9424,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -9424,7 +9433,7 @@
       <c r="C18" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="4"/>
       <c r="F18" s="0" t="s">
         <v>267</v>
       </c>
@@ -9433,7 +9442,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B19" s="0" t="s">
@@ -9442,7 +9451,7 @@
       <c r="C19" s="0" t="s">
         <v>387</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F19" s="0" t="s">
@@ -9453,7 +9462,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B20" s="0" t="s">
@@ -9462,7 +9471,7 @@
       <c r="C20" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F20" s="0" t="s">
@@ -9473,7 +9482,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B21" s="0" t="s">
@@ -9490,7 +9499,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -9499,7 +9508,7 @@
       <c r="C22" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F22" s="0" t="s">
@@ -9510,7 +9519,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -9519,7 +9528,7 @@
       <c r="C23" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F23" s="0" t="s">
@@ -9530,7 +9539,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B24" s="0" t="s">
@@ -9539,7 +9548,7 @@
       <c r="C24" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F24" s="0" t="s">
@@ -9550,7 +9559,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B25" s="0" t="s">
@@ -9559,7 +9568,7 @@
       <c r="C25" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F25" s="0" t="s">
@@ -9570,7 +9579,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="4" t="n">
         <v>42200</v>
       </c>
       <c r="B26" s="0" t="s">
@@ -9579,7 +9588,7 @@
       <c r="C26" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="4" t="n">
         <v>42207</v>
       </c>
       <c r="F26" s="0" t="s">
@@ -9607,7 +9616,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -9637,7 +9646,7 @@
         <v>604</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>297</v>
+        <v>605</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>301</v>
@@ -9648,16 +9657,16 @@
         <v>277</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>42114</v>
@@ -9668,13 +9677,13 @@
         <v>277</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>610</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>609</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>608</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>42128</v>
@@ -9685,13 +9694,13 @@
         <v>277</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>42128</v>
@@ -9702,13 +9711,13 @@
         <v>277</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>42128</v>
@@ -9719,13 +9728,13 @@
         <v>277</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>42128</v>
@@ -9736,13 +9745,13 @@
         <v>277</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>42128</v>
@@ -9753,13 +9762,13 @@
         <v>277</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>615</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>614</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>42128</v>
@@ -9770,13 +9779,13 @@
         <v>277</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>42128</v>
@@ -9787,13 +9796,13 @@
         <v>277</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>618</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>617</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>42128</v>
@@ -9804,13 +9813,13 @@
         <v>277</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>42090</v>
@@ -9821,13 +9830,13 @@
         <v>277</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>42142</v>
@@ -9838,13 +9847,13 @@
         <v>277</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>623</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>622</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>42142</v>
@@ -9855,13 +9864,13 @@
         <v>277</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>42150</v>
@@ -9872,13 +9881,13 @@
         <v>277</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>42177</v>
@@ -9889,13 +9898,13 @@
         <v>277</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>42121</v>
@@ -9906,13 +9915,13 @@
         <v>277</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>42150</v>
@@ -9923,13 +9932,13 @@
         <v>277</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>42159</v>
@@ -9940,13 +9949,13 @@
         <v>277</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>42159</v>
@@ -9957,13 +9966,13 @@
         <v>277</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>42159</v>
@@ -9974,13 +9983,13 @@
         <v>277</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>42080</v>
@@ -9991,13 +10000,13 @@
         <v>277</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>635</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>634</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>633</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>42192</v>
@@ -10011,13 +10020,13 @@
         <v>277</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>42192</v>
@@ -10031,13 +10040,13 @@
         <v>277</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>42192</v>
@@ -10051,10 +10060,10 @@
         <v>277</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>12</v>
@@ -10071,13 +10080,13 @@
         <v>277</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>42101</v>
@@ -10088,13 +10097,13 @@
         <v>277</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>42080</v>
@@ -10105,13 +10114,13 @@
         <v>277</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F28" s="2" t="n">
         <v>42080</v>
@@ -10122,13 +10131,13 @@
         <v>277</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>42032</v>
@@ -10139,13 +10148,13 @@
         <v>277</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>42101</v>
@@ -10169,7 +10178,7 @@
   </sheetPr>
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -10180,37 +10189,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>